<commit_message>
Issue #25. Update the test xlsx manifest files (both the good ones and the bad ones) to have valid entries in the 'Language' and 'Topical Subject' columns. This fixes all of the batch ingest tests. (Still need to add a couple of tests with missing language and topical subject.)
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/badName_required_column.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/badName_required_column.xlsx
@@ -5,91 +5,105 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
-  <si>
-    <t>Bad Name for Required Column</t>
-  </si>
-  <si>
-    <t>frances.dickens@reichel.com</t>
-  </si>
-  <si>
-    <t>Main Tootle</t>
-  </si>
-  <si>
-    <t>Contributor</t>
-  </si>
-  <si>
-    <t>Genre</t>
-  </si>
-  <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>Date Created</t>
-  </si>
-  <si>
-    <t>Date Issued</t>
-  </si>
-  <si>
-    <t>Abstract</t>
-  </si>
-  <si>
-    <t>Topical Subject</t>
-  </si>
-  <si>
-    <t>Geographic Subject</t>
-  </si>
-  <si>
-    <t>Temporal Subject</t>
-  </si>
-  <si>
-    <t>Publish</t>
-  </si>
-  <si>
-    <t>Hidden</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Offset</t>
-  </si>
-  <si>
-    <t>Skip Transcoding</t>
-  </si>
-  <si>
-    <t>Absolute Location</t>
-  </si>
-  <si>
-    <t>Test Batch - File 1 with space</t>
-  </si>
-  <si>
-    <t>Julie Hardesty</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>content/0276 med.mp4</t>
-  </si>
-  <si>
-    <t>Test Batch - File 2 with space</t>
-  </si>
-  <si>
-    <t>content/tone loc.wav</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">Bad Name for Required Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frances.dickens@reichel.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Tootle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Issued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topical Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geographic Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporal Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skip Transcoding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Batch - File 1 with space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julie Hardesty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content/0276 med.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Batch - File 2 with space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content/tone loc.wav</t>
   </si>
 </sst>
 </file>
@@ -97,7 +111,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -231,29 +245,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.4925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.4925925925926"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.8296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="10.8333333333333"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.4925925925926"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.837037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.4925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,45 +332,63 @@
       <c r="Q2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="R2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>